<commit_message>
Set default position to A1
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_500k_increase_1m_decrease.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_500k_increase_1m_decrease.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Documents\edited_town_close_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0BC583A-E5E5-421E-8047-D989B1BEC683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52819A1B-7DC0-4B3B-9277-DFFBC3C5D76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88247574-0E85-40E1-B23C-5A7835C1E323}"/>
+    <workbookView xWindow="-33945" yWindow="4005" windowWidth="27765" windowHeight="9525" xr2:uid="{88247574-0E85-40E1-B23C-5A7835C1E323}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -496,9 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF9AA25-C6AE-4B99-9325-6A04FA17227B}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Update town close year columns (#769)
* Fix filter generation on table

* Update columns

* Revert changes

* Revert file

* Revert file

* Revert file

* Fix column widths

* Continue to add PR feedback

* Extend column width

* Update dbt/scripts/utils/export.py

Co-authored-by: Jean Cochrane <jeancochrane@users.noreply.github.com>

* Set default position to A1

* Declutter column widths

* Switch current year to prior year on wrong columns

---------

Co-authored-by: Jean Cochrane <jeancochrane@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_report_town_close_500k_increase_1m_decrease.xlsx
+++ b/dbt/export/templates/qc.vw_report_town_close_500k_increase_1m_decrease.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miwagne\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C1455D-0E77-4A53-9E74-27D4C28914B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D182731F-B17C-42EE-9FEF-0CD9FBCA7D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="1935" windowWidth="21600" windowHeight="11295" xr2:uid="{88247574-0E85-40E1-B23C-5A7835C1E323}"/>
+    <workbookView xWindow="-33945" yWindow="4005" windowWidth="27765" windowHeight="9525" xr2:uid="{88247574-0E85-40E1-B23C-5A7835C1E323}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -56,34 +56,34 @@
     <t>REASCD</t>
   </si>
   <si>
-    <t>2023 LMV</t>
-  </si>
-  <si>
-    <t>2023 BMV</t>
-  </si>
-  <si>
-    <t>2023 Total</t>
-  </si>
-  <si>
     <t>DIFFERENCE</t>
   </si>
   <si>
     <t>% Change</t>
   </si>
   <si>
-    <t>2024 LMV</t>
-  </si>
-  <si>
-    <t>2024 BMV</t>
-  </si>
-  <si>
-    <t>2024 Total</t>
-  </si>
-  <si>
     <t>TOWNSHIP</t>
   </si>
   <si>
     <t>TAXYR</t>
+  </si>
+  <si>
+    <t>Prior Year LMV</t>
+  </si>
+  <si>
+    <t>Prior Year BMV</t>
+  </si>
+  <si>
+    <t>Prior Year Total</t>
+  </si>
+  <si>
+    <t>Curr. Year LMV</t>
+  </si>
+  <si>
+    <t>Curr. Year BMV</t>
+  </si>
+  <si>
+    <t>Curr. Year Total</t>
   </si>
 </sst>
 </file>
@@ -198,9 +198,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -238,7 +238,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -344,7 +344,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -486,7 +486,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,37 +496,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF9AA25-C6AE-4B99-9325-6A04FA17227B}">
   <dimension ref="A1:P1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -535,28 +535,28 @@
         <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>1</v>

</xml_diff>